<commit_message>
update smart farm datamart
</commit_message>
<xml_diff>
--- a/df_cropping.xlsx
+++ b/df_cropping.xlsx
@@ -611,7 +611,7 @@
         <v>4</v>
       </c>
       <c r="P2" t="n">
-        <v>2.5</v>
+        <v>2.44</v>
       </c>
       <c r="Q2" t="n">
         <v>2.5</v>
@@ -817,7 +817,7 @@
         <v>4</v>
       </c>
       <c r="P5" t="n">
-        <v>2.5</v>
+        <v>2.37</v>
       </c>
       <c r="Q5" t="n">
         <v>2.5</v>
@@ -901,13 +901,13 @@
         <v>3</v>
       </c>
       <c r="N6" t="n">
+        <v>4</v>
+      </c>
+      <c r="O6" t="n">
         <v>2</v>
       </c>
-      <c r="O6" t="n">
-        <v>4</v>
-      </c>
       <c r="P6" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="Q6" t="n">
         <v>2.5</v>
@@ -997,7 +997,7 @@
         <v>5</v>
       </c>
       <c r="P7" t="n">
-        <v>2.5</v>
+        <v>2.36</v>
       </c>
       <c r="Q7" t="n">
         <v>2.5</v>
@@ -1087,7 +1087,7 @@
         <v>5</v>
       </c>
       <c r="P8" t="n">
-        <v>2.5</v>
+        <v>6.32</v>
       </c>
       <c r="Q8" t="n">
         <v>2.5</v>
@@ -1177,7 +1177,7 @@
         <v>2</v>
       </c>
       <c r="P9" t="n">
-        <v>6.8</v>
+        <v>2.23</v>
       </c>
       <c r="Q9" t="n">
         <v>6.8</v>
@@ -1267,7 +1267,7 @@
         <v>5</v>
       </c>
       <c r="P10" t="n">
-        <v>2.5</v>
+        <v>2.83</v>
       </c>
       <c r="Q10" t="n">
         <v>2.5</v>
@@ -1357,7 +1357,7 @@
         <v>4</v>
       </c>
       <c r="P11" t="n">
-        <v>6.8</v>
+        <v>2.51</v>
       </c>
       <c r="Q11" t="n">
         <v>6.8</v>
@@ -1845,7 +1845,7 @@
         <v>6</v>
       </c>
       <c r="P19" t="n">
-        <v>6.8</v>
+        <v>2.52</v>
       </c>
       <c r="Q19" t="n">
         <v>6.8</v>
@@ -1928,9 +1928,7 @@
       </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
-      <c r="P20" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P20" t="inlineStr"/>
       <c r="Q20" t="n">
         <v>2.5</v>
       </c>
@@ -2013,7 +2011,7 @@
         <v>5</v>
       </c>
       <c r="P21" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q21" t="n">
         <v>2.5</v>
@@ -2159,7 +2157,7 @@
         <v>5</v>
       </c>
       <c r="P23" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q23" t="n">
         <v>2.5</v>
@@ -2240,9 +2238,7 @@
       <c r="O24" t="n">
         <v>5</v>
       </c>
-      <c r="P24" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P24" t="inlineStr"/>
       <c r="Q24" t="n">
         <v>2.5</v>
       </c>
@@ -2331,7 +2327,7 @@
         <v>5</v>
       </c>
       <c r="P25" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q25" t="n">
         <v>2.5</v>
@@ -2413,7 +2409,7 @@
         <v>5</v>
       </c>
       <c r="P26" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q26" t="n">
         <v>2.5</v>
@@ -2503,7 +2499,7 @@
         <v>5</v>
       </c>
       <c r="P27" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q27" t="n">
         <v>2.5</v>
@@ -2585,7 +2581,7 @@
         <v>5</v>
       </c>
       <c r="P28" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q28" t="n">
         <v>2.5</v>
@@ -2675,7 +2671,7 @@
         <v>5</v>
       </c>
       <c r="P29" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q29" t="n">
         <v>2.5</v>
@@ -2765,7 +2761,7 @@
         <v>5</v>
       </c>
       <c r="P30" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q30" t="n">
         <v>2.5</v>
@@ -2847,7 +2843,7 @@
         <v>5</v>
       </c>
       <c r="P31" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q31" t="n">
         <v>2.5</v>
@@ -2937,7 +2933,7 @@
         <v>5</v>
       </c>
       <c r="P32" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q32" t="n">
         <v>2.5</v>
@@ -3027,7 +3023,7 @@
         <v>5</v>
       </c>
       <c r="P33" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q33" t="n">
         <v>2.5</v>
@@ -3175,7 +3171,7 @@
         <v>5</v>
       </c>
       <c r="P35" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q35" t="n">
         <v>2.5</v>
@@ -3257,7 +3253,7 @@
         <v>5</v>
       </c>
       <c r="P36" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q36" t="n">
         <v>2.5</v>
@@ -3405,7 +3401,7 @@
         <v>5</v>
       </c>
       <c r="P38" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q38" t="n">
         <v>2.5</v>
@@ -3487,7 +3483,7 @@
         <v>5</v>
       </c>
       <c r="P39" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q39" t="n">
         <v>2.5</v>
@@ -3569,7 +3565,7 @@
         <v>5</v>
       </c>
       <c r="P40" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q40" t="n">
         <v>2.5</v>
@@ -3659,7 +3655,7 @@
         <v>5</v>
       </c>
       <c r="P41" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q41" t="n">
         <v>2.5</v>
@@ -3749,7 +3745,7 @@
         <v>5</v>
       </c>
       <c r="P42" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q42" t="n">
         <v>2.5</v>
@@ -3839,7 +3835,7 @@
         <v>5</v>
       </c>
       <c r="P43" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q43" t="n">
         <v>2.5</v>
@@ -3921,7 +3917,7 @@
         <v>5</v>
       </c>
       <c r="P44" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q44" t="n">
         <v>2.5</v>
@@ -4011,7 +4007,7 @@
         <v>5</v>
       </c>
       <c r="P45" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q45" t="n">
         <v>2.5</v>
@@ -4092,9 +4088,7 @@
       <c r="O46" t="n">
         <v>5</v>
       </c>
-      <c r="P46" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P46" t="inlineStr"/>
       <c r="Q46" t="n">
         <v>2.5</v>
       </c>
@@ -4181,7 +4175,7 @@
         <v>5</v>
       </c>
       <c r="P47" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q47" t="n">
         <v>2.5</v>
@@ -4263,7 +4257,7 @@
         <v>5</v>
       </c>
       <c r="P48" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q48" t="n">
         <v>2.5</v>
@@ -4353,7 +4347,7 @@
         <v>5</v>
       </c>
       <c r="P49" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q49" t="n">
         <v>2.5</v>
@@ -4435,7 +4429,7 @@
         <v>5</v>
       </c>
       <c r="P50" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q50" t="n">
         <v>2.5</v>
@@ -4525,7 +4519,7 @@
         <v>5</v>
       </c>
       <c r="P51" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q51" t="n">
         <v>2.5</v>
@@ -4731,7 +4725,7 @@
         <v>4</v>
       </c>
       <c r="P54" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q54" t="n">
         <v>2.5</v>
@@ -4821,7 +4815,7 @@
         <v>4</v>
       </c>
       <c r="P55" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q55" t="n">
         <v>2.5</v>
@@ -4911,7 +4905,7 @@
         <v>5</v>
       </c>
       <c r="P56" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q56" t="n">
         <v>2.5</v>
@@ -5001,7 +4995,7 @@
         <v>5</v>
       </c>
       <c r="P57" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q57" t="n">
         <v>2.5</v>
@@ -5149,7 +5143,7 @@
         <v>5</v>
       </c>
       <c r="P59" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q59" t="n">
         <v>2.5</v>
@@ -5467,7 +5461,7 @@
         <v>5</v>
       </c>
       <c r="P64" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q64" t="n">
         <v>2.5</v>
@@ -5536,9 +5530,7 @@
       <c r="M65" t="inlineStr"/>
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
-      <c r="P65" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P65" t="inlineStr"/>
       <c r="Q65" t="n">
         <v>2.5</v>
       </c>
@@ -5959,7 +5951,7 @@
         <v>5</v>
       </c>
       <c r="P72" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q72" t="n">
         <v>2.5</v>
@@ -6268,9 +6260,7 @@
       <c r="M77" t="inlineStr"/>
       <c r="N77" t="inlineStr"/>
       <c r="O77" t="inlineStr"/>
-      <c r="P77" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P77" t="inlineStr"/>
       <c r="Q77" t="n">
         <v>2.5</v>
       </c>
@@ -6562,9 +6552,7 @@
       <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="inlineStr"/>
-      <c r="P82" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P82" t="inlineStr"/>
       <c r="Q82" t="n">
         <v>2.5</v>
       </c>
@@ -6927,7 +6915,7 @@
         <v>5</v>
       </c>
       <c r="P88" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q88" t="n">
         <v>2.5</v>
@@ -7009,7 +6997,7 @@
         <v>5</v>
       </c>
       <c r="P89" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q89" t="n">
         <v>2.5</v>
@@ -9058,9 +9046,7 @@
       </c>
       <c r="N123" t="inlineStr"/>
       <c r="O123" t="inlineStr"/>
-      <c r="P123" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P123" t="inlineStr"/>
       <c r="Q123" t="n">
         <v>2.5</v>
       </c>
@@ -9304,9 +9290,7 @@
       </c>
       <c r="N127" t="inlineStr"/>
       <c r="O127" t="inlineStr"/>
-      <c r="P127" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P127" t="inlineStr"/>
       <c r="Q127" t="n">
         <v>2.5</v>
       </c>
@@ -9985,7 +9969,7 @@
         <v>5</v>
       </c>
       <c r="P138" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q138" t="n">
         <v>2.5</v>
@@ -10707,7 +10691,7 @@
         <v>5</v>
       </c>
       <c r="P150" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q150" t="n">
         <v>2.5</v>
@@ -11020,9 +11004,7 @@
       <c r="M155" t="inlineStr"/>
       <c r="N155" t="inlineStr"/>
       <c r="O155" t="inlineStr"/>
-      <c r="P155" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P155" t="inlineStr"/>
       <c r="Q155" t="n">
         <v>2.5</v>
       </c>
@@ -11556,9 +11538,7 @@
       </c>
       <c r="N164" t="inlineStr"/>
       <c r="O164" t="inlineStr"/>
-      <c r="P164" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P164" t="inlineStr"/>
       <c r="Q164" t="n">
         <v>2.5</v>
       </c>
@@ -12518,9 +12498,7 @@
       <c r="M180" t="inlineStr"/>
       <c r="N180" t="inlineStr"/>
       <c r="O180" t="inlineStr"/>
-      <c r="P180" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P180" t="inlineStr"/>
       <c r="Q180" t="n">
         <v>2.5</v>
       </c>
@@ -13586,9 +13564,7 @@
       <c r="M198" t="inlineStr"/>
       <c r="N198" t="inlineStr"/>
       <c r="O198" t="inlineStr"/>
-      <c r="P198" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P198" t="inlineStr"/>
       <c r="Q198" t="n">
         <v>2.5</v>
       </c>
@@ -13996,9 +13972,7 @@
       <c r="M205" t="inlineStr"/>
       <c r="N205" t="inlineStr"/>
       <c r="O205" t="inlineStr"/>
-      <c r="P205" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P205" t="inlineStr"/>
       <c r="Q205" t="n">
         <v>2.5</v>
       </c>
@@ -14599,7 +14573,7 @@
         <v>5</v>
       </c>
       <c r="P215" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q215" t="n">
         <v>2.5</v>
@@ -15270,9 +15244,7 @@
       <c r="M226" t="inlineStr"/>
       <c r="N226" t="inlineStr"/>
       <c r="O226" t="inlineStr"/>
-      <c r="P226" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P226" t="inlineStr"/>
       <c r="Q226" t="n">
         <v>2.5</v>
       </c>
@@ -16411,7 +16383,7 @@
         <v>5</v>
       </c>
       <c r="P245" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q245" t="n">
         <v>2.5</v>
@@ -16501,7 +16473,7 @@
         <v>5</v>
       </c>
       <c r="P246" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q246" t="n">
         <v>2.5</v>
@@ -16591,7 +16563,7 @@
         <v>5</v>
       </c>
       <c r="P247" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q247" t="n">
         <v>2.5</v>
@@ -16681,7 +16653,7 @@
         <v>5</v>
       </c>
       <c r="P248" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q248" t="n">
         <v>2.5</v>
@@ -16887,7 +16859,7 @@
         <v>5</v>
       </c>
       <c r="P251" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q251" t="n">
         <v>2.5</v>
@@ -17035,7 +17007,7 @@
         <v>5</v>
       </c>
       <c r="P253" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q253" t="n">
         <v>2.5</v>
@@ -17179,7 +17151,7 @@
         <v>5</v>
       </c>
       <c r="P255" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q255" t="n">
         <v>2.5</v>
@@ -17261,7 +17233,7 @@
         <v>5</v>
       </c>
       <c r="P256" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q256" t="n">
         <v>2.5</v>
@@ -18214,9 +18186,7 @@
       </c>
       <c r="N272" t="inlineStr"/>
       <c r="O272" t="inlineStr"/>
-      <c r="P272" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P272" t="inlineStr"/>
       <c r="Q272" t="n">
         <v>2.5</v>
       </c>
@@ -18348,9 +18318,7 @@
       </c>
       <c r="N274" t="inlineStr"/>
       <c r="O274" t="inlineStr"/>
-      <c r="P274" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P274" t="inlineStr"/>
       <c r="Q274" t="n">
         <v>2.5</v>
       </c>
@@ -19082,9 +19050,7 @@
       </c>
       <c r="N286" t="inlineStr"/>
       <c r="O286" t="inlineStr"/>
-      <c r="P286" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P286" t="inlineStr"/>
       <c r="Q286" t="n">
         <v>2.5</v>
       </c>
@@ -19146,9 +19112,7 @@
       </c>
       <c r="N287" t="inlineStr"/>
       <c r="O287" t="inlineStr"/>
-      <c r="P287" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P287" t="inlineStr"/>
       <c r="Q287" t="n">
         <v>2.5</v>
       </c>
@@ -19500,9 +19464,7 @@
       </c>
       <c r="N293" t="inlineStr"/>
       <c r="O293" t="inlineStr"/>
-      <c r="P293" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P293" t="inlineStr"/>
       <c r="Q293" t="n">
         <v>2.5</v>
       </c>
@@ -19684,9 +19646,7 @@
       </c>
       <c r="N296" t="inlineStr"/>
       <c r="O296" t="inlineStr"/>
-      <c r="P296" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P296" t="inlineStr"/>
       <c r="Q296" t="n">
         <v>2.5</v>
       </c>
@@ -19756,9 +19716,7 @@
       </c>
       <c r="N297" t="inlineStr"/>
       <c r="O297" t="inlineStr"/>
-      <c r="P297" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P297" t="inlineStr"/>
       <c r="Q297" t="n">
         <v>2.5</v>
       </c>
@@ -19880,9 +19838,7 @@
       <c r="M299" t="inlineStr"/>
       <c r="N299" t="inlineStr"/>
       <c r="O299" t="inlineStr"/>
-      <c r="P299" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P299" t="inlineStr"/>
       <c r="Q299" t="n">
         <v>2.5</v>
       </c>
@@ -20232,9 +20188,7 @@
       <c r="M305" t="inlineStr"/>
       <c r="N305" t="inlineStr"/>
       <c r="O305" t="inlineStr"/>
-      <c r="P305" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P305" t="inlineStr"/>
       <c r="Q305" t="n">
         <v>2.5</v>
       </c>
@@ -20716,9 +20670,7 @@
       </c>
       <c r="N313" t="inlineStr"/>
       <c r="O313" t="inlineStr"/>
-      <c r="P313" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P313" t="inlineStr"/>
       <c r="Q313" t="n">
         <v>2.5</v>
       </c>
@@ -20790,9 +20742,7 @@
       </c>
       <c r="N314" t="inlineStr"/>
       <c r="O314" t="inlineStr"/>
-      <c r="P314" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P314" t="inlineStr"/>
       <c r="Q314" t="n">
         <v>2.5</v>
       </c>
@@ -21030,9 +20980,7 @@
       <c r="M318" t="inlineStr"/>
       <c r="N318" t="inlineStr"/>
       <c r="O318" t="inlineStr"/>
-      <c r="P318" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P318" t="inlineStr"/>
       <c r="Q318" t="n">
         <v>2.5</v>
       </c>
@@ -21332,9 +21280,7 @@
       <c r="M323" t="inlineStr"/>
       <c r="N323" t="inlineStr"/>
       <c r="O323" t="inlineStr"/>
-      <c r="P323" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P323" t="inlineStr"/>
       <c r="Q323" t="n">
         <v>2.5</v>
       </c>
@@ -21916,9 +21862,7 @@
       <c r="M333" t="inlineStr"/>
       <c r="N333" t="inlineStr"/>
       <c r="O333" t="inlineStr"/>
-      <c r="P333" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P333" t="inlineStr"/>
       <c r="Q333" t="n">
         <v>2.5</v>
       </c>
@@ -22380,9 +22324,7 @@
       <c r="M341" t="inlineStr"/>
       <c r="N341" t="inlineStr"/>
       <c r="O341" t="inlineStr"/>
-      <c r="P341" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P341" t="inlineStr"/>
       <c r="Q341" t="n">
         <v>2.5</v>
       </c>
@@ -22736,9 +22678,7 @@
       <c r="M347" t="inlineStr"/>
       <c r="N347" t="inlineStr"/>
       <c r="O347" t="inlineStr"/>
-      <c r="P347" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P347" t="inlineStr"/>
       <c r="Q347" t="n">
         <v>2.5</v>
       </c>
@@ -22916,9 +22856,7 @@
       </c>
       <c r="N350" t="inlineStr"/>
       <c r="O350" t="inlineStr"/>
-      <c r="P350" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P350" t="inlineStr"/>
       <c r="Q350" t="n">
         <v>2.5</v>
       </c>
@@ -78663,7 +78601,7 @@
         <v>5</v>
       </c>
       <c r="P1267" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1267" t="n">
         <v>2.5</v>
@@ -78753,7 +78691,7 @@
         <v>5</v>
       </c>
       <c r="P1268" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1268" t="n">
         <v>2.5</v>
@@ -78901,7 +78839,7 @@
         <v>5</v>
       </c>
       <c r="P1270" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1270" t="n">
         <v>2.5</v>
@@ -78991,7 +78929,7 @@
         <v>5</v>
       </c>
       <c r="P1271" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1271" t="n">
         <v>2.5</v>
@@ -79081,7 +79019,7 @@
         <v>5</v>
       </c>
       <c r="P1272" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1272" t="n">
         <v>2.5</v>
@@ -79171,7 +79109,7 @@
         <v>5</v>
       </c>
       <c r="P1273" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1273" t="n">
         <v>2.5</v>
@@ -79261,7 +79199,7 @@
         <v>5</v>
       </c>
       <c r="P1274" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1274" t="n">
         <v>2.5</v>
@@ -79351,7 +79289,7 @@
         <v>5</v>
       </c>
       <c r="P1275" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1275" t="n">
         <v>2.5</v>
@@ -79441,7 +79379,7 @@
         <v>5</v>
       </c>
       <c r="P1276" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1276" t="n">
         <v>2.5</v>
@@ -79531,7 +79469,7 @@
         <v>5</v>
       </c>
       <c r="P1277" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1277" t="n">
         <v>2.5</v>
@@ -79621,7 +79559,7 @@
         <v>5</v>
       </c>
       <c r="P1278" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1278" t="n">
         <v>2.5</v>
@@ -79711,7 +79649,7 @@
         <v>5</v>
       </c>
       <c r="P1279" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1279" t="n">
         <v>2.5</v>
@@ -79801,7 +79739,7 @@
         <v>5</v>
       </c>
       <c r="P1280" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1280" t="n">
         <v>2.5</v>
@@ -79891,7 +79829,7 @@
         <v>5</v>
       </c>
       <c r="P1281" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1281" t="n">
         <v>2.5</v>
@@ -79981,7 +79919,7 @@
         <v>5</v>
       </c>
       <c r="P1282" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1282" t="n">
         <v>2.5</v>
@@ -80062,9 +80000,7 @@
       <c r="O1283" t="n">
         <v>5</v>
       </c>
-      <c r="P1283" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="P1283" t="inlineStr"/>
       <c r="Q1283" t="n">
         <v>2.5</v>
       </c>
@@ -80281,7 +80217,7 @@
         <v>5</v>
       </c>
       <c r="P1286" t="n">
-        <v>2.5</v>
+        <v>2.73</v>
       </c>
       <c r="Q1286" t="n">
         <v>2.5</v>

</xml_diff>